<commit_message>
fix something + try js in project
</commit_message>
<xml_diff>
--- a/plan.xlsx
+++ b/plan.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\projectWeb\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5032B94-CCBC-430B-9419-982D46C43059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="28755" windowHeight="12600"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -63,18 +69,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -89,6 +87,13 @@
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -141,24 +146,24 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -166,6 +171,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -212,7 +225,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -244,9 +257,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -278,6 +309,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -453,97 +502,120 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:D7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="4" width="31" customWidth="1"/>
     <col min="5" max="5" width="25.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" ht="21">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="111" customHeight="1">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:4" ht="111" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="75">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:4" ht="93.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="37.5">
-      <c r="A5" s="5" t="s">
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="1:4" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="1:4" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="1" t="s">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:4" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
         <v>11</v>
       </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>